<commit_message>
se harán nuevos algoritmos para todo lo global
</commit_message>
<xml_diff>
--- a/Compresion.xlsx
+++ b/Compresion.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A1679"/>
+  <dimension ref="A1:A1751"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -8830,6 +8830,366 @@
         <v>0.338409475465313</v>
       </c>
     </row>
+    <row r="1680">
+      <c r="A1680" t="n">
+        <v>0.338409475465313</v>
+      </c>
+    </row>
+    <row r="1681">
+      <c r="A1681" t="n">
+        <v>0.338409475465313</v>
+      </c>
+    </row>
+    <row r="1682">
+      <c r="A1682" t="n">
+        <v>0.338409475465313</v>
+      </c>
+    </row>
+    <row r="1683">
+      <c r="A1683" t="n">
+        <v>0.338409475465313</v>
+      </c>
+    </row>
+    <row r="1684">
+      <c r="A1684" t="n">
+        <v>0.338409475465313</v>
+      </c>
+    </row>
+    <row r="1685">
+      <c r="A1685" t="n">
+        <v>0.338409475465313</v>
+      </c>
+    </row>
+    <row r="1686">
+      <c r="A1686" t="n">
+        <v>0.338409475465313</v>
+      </c>
+    </row>
+    <row r="1687">
+      <c r="A1687" t="n">
+        <v>0.338409475465313</v>
+      </c>
+    </row>
+    <row r="1688">
+      <c r="A1688" t="n">
+        <v>0.338409475465313</v>
+      </c>
+    </row>
+    <row r="1689">
+      <c r="A1689" t="n">
+        <v>0.338409475465313</v>
+      </c>
+    </row>
+    <row r="1690">
+      <c r="A1690" t="n">
+        <v>0.338409475465313</v>
+      </c>
+    </row>
+    <row r="1691">
+      <c r="A1691" t="n">
+        <v>0.338409475465313</v>
+      </c>
+    </row>
+    <row r="1692">
+      <c r="A1692" t="n">
+        <v>0.338409475465313</v>
+      </c>
+    </row>
+    <row r="1693">
+      <c r="A1693" t="n">
+        <v>0.338409475465313</v>
+      </c>
+    </row>
+    <row r="1694">
+      <c r="A1694" t="n">
+        <v>0.338409475465313</v>
+      </c>
+    </row>
+    <row r="1695">
+      <c r="A1695" t="n">
+        <v>0.338409475465313</v>
+      </c>
+    </row>
+    <row r="1696">
+      <c r="A1696" t="n">
+        <v>0.338409475465313</v>
+      </c>
+    </row>
+    <row r="1697">
+      <c r="A1697" t="n">
+        <v>0.338409475465313</v>
+      </c>
+    </row>
+    <row r="1698">
+      <c r="A1698" t="n">
+        <v>0.338409475465313</v>
+      </c>
+    </row>
+    <row r="1699">
+      <c r="A1699" t="n">
+        <v>0.338409475465313</v>
+      </c>
+    </row>
+    <row r="1700">
+      <c r="A1700" t="n">
+        <v>0.338409475465313</v>
+      </c>
+    </row>
+    <row r="1701">
+      <c r="A1701" t="n">
+        <v>0.338409475465313</v>
+      </c>
+    </row>
+    <row r="1702">
+      <c r="A1702" t="n">
+        <v>0.338409475465313</v>
+      </c>
+    </row>
+    <row r="1703">
+      <c r="A1703" t="n">
+        <v>0.338409475465313</v>
+      </c>
+    </row>
+    <row r="1704">
+      <c r="A1704" t="n">
+        <v>0.338409475465313</v>
+      </c>
+    </row>
+    <row r="1705">
+      <c r="A1705" t="n">
+        <v>0.338409475465313</v>
+      </c>
+    </row>
+    <row r="1706">
+      <c r="A1706" t="n">
+        <v>0.338409475465313</v>
+      </c>
+    </row>
+    <row r="1707">
+      <c r="A1707" t="n">
+        <v>0.338409475465313</v>
+      </c>
+    </row>
+    <row r="1708">
+      <c r="A1708" t="n">
+        <v>0.338409475465313</v>
+      </c>
+    </row>
+    <row r="1709">
+      <c r="A1709" t="n">
+        <v>0.338409475465313</v>
+      </c>
+    </row>
+    <row r="1710">
+      <c r="A1710" t="n">
+        <v>0.338409475465313</v>
+      </c>
+    </row>
+    <row r="1711">
+      <c r="A1711" t="n">
+        <v>0.338409475465313</v>
+      </c>
+    </row>
+    <row r="1712">
+      <c r="A1712" t="n">
+        <v>0.338409475465313</v>
+      </c>
+    </row>
+    <row r="1713">
+      <c r="A1713" t="n">
+        <v>0.338409475465313</v>
+      </c>
+    </row>
+    <row r="1714">
+      <c r="A1714" t="n">
+        <v>0.338409475465313</v>
+      </c>
+    </row>
+    <row r="1715">
+      <c r="A1715" t="n">
+        <v>0.338409475465313</v>
+      </c>
+    </row>
+    <row r="1716">
+      <c r="A1716" t="n">
+        <v>0.338409475465313</v>
+      </c>
+    </row>
+    <row r="1717">
+      <c r="A1717" t="n">
+        <v>0.338409475465313</v>
+      </c>
+    </row>
+    <row r="1718">
+      <c r="A1718" t="n">
+        <v>0.338409475465313</v>
+      </c>
+    </row>
+    <row r="1719">
+      <c r="A1719" t="n">
+        <v>0.338409475465313</v>
+      </c>
+    </row>
+    <row r="1720">
+      <c r="A1720" t="n">
+        <v>0.338409475465313</v>
+      </c>
+    </row>
+    <row r="1721">
+      <c r="A1721" t="n">
+        <v>0.338409475465313</v>
+      </c>
+    </row>
+    <row r="1722">
+      <c r="A1722" t="n">
+        <v>0.338409475465313</v>
+      </c>
+    </row>
+    <row r="1723">
+      <c r="A1723" t="n">
+        <v>0.338409475465313</v>
+      </c>
+    </row>
+    <row r="1724">
+      <c r="A1724" t="n">
+        <v>0.338409475465313</v>
+      </c>
+    </row>
+    <row r="1725">
+      <c r="A1725" t="n">
+        <v>0.338409475465313</v>
+      </c>
+    </row>
+    <row r="1726">
+      <c r="A1726" t="n">
+        <v>0.338409475465313</v>
+      </c>
+    </row>
+    <row r="1727">
+      <c r="A1727" t="n">
+        <v>0.338409475465313</v>
+      </c>
+    </row>
+    <row r="1728">
+      <c r="A1728" t="n">
+        <v>0.338409475465313</v>
+      </c>
+    </row>
+    <row r="1729">
+      <c r="A1729" t="n">
+        <v>0.338409475465313</v>
+      </c>
+    </row>
+    <row r="1730">
+      <c r="A1730" t="n">
+        <v>0.338409475465313</v>
+      </c>
+    </row>
+    <row r="1731">
+      <c r="A1731" t="n">
+        <v>0.338409475465313</v>
+      </c>
+    </row>
+    <row r="1732">
+      <c r="A1732" t="n">
+        <v>0.338409475465313</v>
+      </c>
+    </row>
+    <row r="1733">
+      <c r="A1733" t="n">
+        <v>0.338409475465313</v>
+      </c>
+    </row>
+    <row r="1734">
+      <c r="A1734" t="n">
+        <v>0.338409475465313</v>
+      </c>
+    </row>
+    <row r="1735">
+      <c r="A1735" t="n">
+        <v>0.338409475465313</v>
+      </c>
+    </row>
+    <row r="1736">
+      <c r="A1736" t="n">
+        <v>0.338409475465313</v>
+      </c>
+    </row>
+    <row r="1737">
+      <c r="A1737" t="n">
+        <v>0.338409475465313</v>
+      </c>
+    </row>
+    <row r="1738">
+      <c r="A1738" t="n">
+        <v>0.338409475465313</v>
+      </c>
+    </row>
+    <row r="1739">
+      <c r="A1739" t="n">
+        <v>0.338409475465313</v>
+      </c>
+    </row>
+    <row r="1740">
+      <c r="A1740" t="n">
+        <v>0.338409475465313</v>
+      </c>
+    </row>
+    <row r="1741">
+      <c r="A1741" t="n">
+        <v>0.338409475465313</v>
+      </c>
+    </row>
+    <row r="1742">
+      <c r="A1742" t="n">
+        <v>0.338409475465313</v>
+      </c>
+    </row>
+    <row r="1743">
+      <c r="A1743" t="n">
+        <v>0.338409475465313</v>
+      </c>
+    </row>
+    <row r="1744">
+      <c r="A1744" t="n">
+        <v>0.338409475465313</v>
+      </c>
+    </row>
+    <row r="1745">
+      <c r="A1745" t="n">
+        <v>0.338409475465313</v>
+      </c>
+    </row>
+    <row r="1746">
+      <c r="A1746" t="n">
+        <v>0.338409475465313</v>
+      </c>
+    </row>
+    <row r="1747">
+      <c r="A1747" t="n">
+        <v>0.338409475465313</v>
+      </c>
+    </row>
+    <row r="1748">
+      <c r="A1748" t="n">
+        <v>0.338409475465313</v>
+      </c>
+    </row>
+    <row r="1749">
+      <c r="A1749" t="n">
+        <v>0.338409475465313</v>
+      </c>
+    </row>
+    <row r="1750">
+      <c r="A1750" t="n">
+        <v>0.338409475465313</v>
+      </c>
+    </row>
+    <row r="1751">
+      <c r="A1751" t="n">
+        <v>0.338409475465313</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>